<commit_message>
Adding playlist upload capability
</commit_message>
<xml_diff>
--- a/excelTest.xlsx
+++ b/excelTest.xlsx
@@ -19,15 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>dave</t>
+    <t>under pressure</t>
   </si>
   <si>
-    <t xml:space="preserve">is </t>
+    <t>david bowie</t>
   </si>
   <si>
-    <t>cool</t>
+    <t>norwegian wood</t>
+  </si>
+  <si>
+    <t>the beatles</t>
   </si>
 </sst>
 </file>
@@ -396,23 +399,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>